<commit_message>
moving around some things
</commit_message>
<xml_diff>
--- a/database/requirements.xlsx
+++ b/database/requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
   <si>
     <t>Item</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>Carnitine</t>
+  </si>
+  <si>
+    <t>Amino acids?</t>
+  </si>
+  <si>
+    <t>Nucleotides?</t>
   </si>
 </sst>
 </file>
@@ -313,12 +319,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,11 +626,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,16 +650,16 @@
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
       <c r="I1" s="2" t="s">
         <v>42</v>
       </c>
@@ -688,14 +694,14 @@
       <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="6"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -704,7 +710,7 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>2500</v>
       </c>
       <c r="D3">
@@ -713,7 +719,7 @@
       <c r="E3">
         <v>2294</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>2000</v>
       </c>
       <c r="G3">
@@ -727,8 +733,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -737,7 +743,7 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>55.5</v>
       </c>
       <c r="D5">
@@ -746,7 +752,7 @@
       <c r="E5">
         <v>53.3</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>45</v>
       </c>
       <c r="G5">
@@ -766,7 +772,7 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>97</v>
       </c>
       <c r="D6">
@@ -775,7 +781,7 @@
       <c r="E6">
         <v>89</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>78</v>
       </c>
       <c r="G6">
@@ -798,7 +804,7 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>31</v>
       </c>
       <c r="D7">
@@ -807,7 +813,7 @@
       <c r="E7">
         <v>28</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>24</v>
       </c>
       <c r="G7">
@@ -830,7 +836,7 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>18</v>
       </c>
       <c r="D8">
@@ -839,7 +845,7 @@
       <c r="E8">
         <v>17</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>14</v>
       </c>
       <c r="G8">
@@ -859,7 +865,7 @@
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>36</v>
       </c>
       <c r="D9">
@@ -868,7 +874,7 @@
       <c r="E9">
         <v>33</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>29</v>
       </c>
       <c r="G9">
@@ -888,7 +894,7 @@
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>333</v>
       </c>
       <c r="D10">
@@ -897,7 +903,7 @@
       <c r="E10">
         <v>306</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>267</v>
       </c>
       <c r="G10">
@@ -917,7 +923,7 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>33</v>
       </c>
       <c r="D11">
@@ -926,7 +932,7 @@
       <c r="E11">
         <v>31</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>27</v>
       </c>
       <c r="G11">
@@ -943,8 +949,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -953,7 +959,7 @@
       <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>6</v>
       </c>
       <c r="D13">
@@ -962,7 +968,7 @@
       <c r="E13">
         <v>6</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>6</v>
       </c>
       <c r="G13">
@@ -985,7 +991,7 @@
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>30</v>
       </c>
       <c r="D14">
@@ -994,7 +1000,7 @@
       <c r="E14">
         <v>30</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>30</v>
       </c>
       <c r="G14">
@@ -1008,8 +1014,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1018,7 +1024,7 @@
       <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>700</v>
       </c>
       <c r="D16">
@@ -1027,7 +1033,7 @@
       <c r="E16">
         <v>700</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>600</v>
       </c>
       <c r="G16">
@@ -1050,7 +1056,7 @@
       <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>1</v>
       </c>
       <c r="D17">
@@ -1059,7 +1065,7 @@
       <c r="E17">
         <v>0.9</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>0.8</v>
       </c>
       <c r="G17">
@@ -1079,7 +1085,7 @@
       <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>1.3</v>
       </c>
       <c r="D18">
@@ -1088,7 +1094,7 @@
       <c r="E18">
         <v>1.3</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>1.1000000000000001</v>
       </c>
       <c r="G18">
@@ -1108,7 +1114,7 @@
       <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>16.5</v>
       </c>
       <c r="D19">
@@ -1117,7 +1123,7 @@
       <c r="E19">
         <v>15.1</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>13.2</v>
       </c>
       <c r="G19">
@@ -1137,8 +1143,8 @@
       <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1147,7 +1153,7 @@
       <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>1.4</v>
       </c>
       <c r="D21">
@@ -1156,7 +1162,7 @@
       <c r="E21">
         <v>1.4</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>1.2</v>
       </c>
       <c r="G21">
@@ -1179,8 +1185,8 @@
       <c r="B22" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="C22" s="6"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1189,7 +1195,7 @@
       <c r="B23" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>200</v>
       </c>
       <c r="D23">
@@ -1198,7 +1204,7 @@
       <c r="E23">
         <v>200</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>200</v>
       </c>
       <c r="G23">
@@ -1218,7 +1224,7 @@
       <c r="B24" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>1.5</v>
       </c>
       <c r="D24">
@@ -1227,7 +1233,7 @@
       <c r="E24">
         <v>1.5</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>1.5</v>
       </c>
       <c r="G24">
@@ -1250,7 +1256,7 @@
       <c r="B25" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>40</v>
       </c>
       <c r="D25">
@@ -1259,7 +1265,7 @@
       <c r="E25">
         <v>40</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>40</v>
       </c>
       <c r="G25">
@@ -1282,7 +1288,7 @@
       <c r="B26" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>10</v>
       </c>
       <c r="D26">
@@ -1291,7 +1297,7 @@
       <c r="E26">
         <v>10</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>10</v>
       </c>
       <c r="G26">
@@ -1317,8 +1323,8 @@
       <c r="B27" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="C27" s="6"/>
+      <c r="F27" s="6"/>
       <c r="J27" t="s">
         <v>65</v>
       </c>
@@ -1330,15 +1336,15 @@
       <c r="B28" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="C28" s="6"/>
+      <c r="F28" s="6"/>
       <c r="J28" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="C29" s="6"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1347,7 +1353,7 @@
       <c r="B30" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>8.6999999999999993</v>
       </c>
       <c r="D30">
@@ -1356,7 +1362,7 @@
       <c r="E30">
         <v>8.6999999999999993</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G30">
@@ -1379,8 +1385,8 @@
       <c r="B31" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="C31" s="6"/>
+      <c r="F31" s="6"/>
       <c r="L31" t="s">
         <v>31</v>
       </c>
@@ -1392,8 +1398,8 @@
       <c r="B32" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="C32" s="6"/>
+      <c r="F32" s="6"/>
       <c r="L32" t="s">
         <v>31</v>
       </c>
@@ -1405,8 +1411,8 @@
       <c r="B33" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="C33" s="6"/>
+      <c r="F33" s="6"/>
       <c r="L33" t="s">
         <v>31</v>
       </c>
@@ -1418,8 +1424,8 @@
       <c r="B34" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="C34" s="6"/>
+      <c r="F34" s="6"/>
       <c r="L34" t="s">
         <v>31</v>
       </c>
@@ -1431,8 +1437,8 @@
       <c r="B35" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="C35" s="6"/>
+      <c r="F35" s="6"/>
       <c r="L35" t="s">
         <v>31</v>
       </c>
@@ -1444,8 +1450,8 @@
       <c r="B36" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="C36" s="6"/>
+      <c r="F36" s="6"/>
       <c r="L36" t="s">
         <v>31</v>
       </c>
@@ -1457,8 +1463,8 @@
       <c r="B37" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="C37" s="6"/>
+      <c r="F37" s="6"/>
       <c r="L37" t="s">
         <v>31</v>
       </c>
@@ -1470,8 +1476,8 @@
       <c r="B38" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="C38" s="6"/>
+      <c r="F38" s="6"/>
       <c r="L38" t="s">
         <v>31</v>
       </c>
@@ -1483,8 +1489,8 @@
       <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="C39" s="6"/>
+      <c r="F39" s="6"/>
       <c r="L39" t="s">
         <v>31</v>
       </c>
@@ -1496,22 +1502,22 @@
       <c r="B40" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="C40" s="6"/>
+      <c r="F40" s="6"/>
       <c r="L40" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="C41" s="6"/>
+      <c r="F41" s="6"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="C42" s="6"/>
+      <c r="F42" s="6"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
@@ -1521,6 +1527,16 @@
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>